<commit_message>
added a few refinements to data analysis as well as background
</commit_message>
<xml_diff>
--- a/survey/UML-Based Development of Large-Scale Dataflow Applications_ Survey (Risposte).xlsx
+++ b/survey/UML-Based Development of Large-Scale Dataflow Applications_ Survey (Risposte).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/streamgen/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4B48476F-C225-224E-B1A5-141AC3ED0358}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{334CC86D-274B-EF4F-BDCB-E2F0A8BE294C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1999,7 +1999,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>